<commit_message>
working build with LDV and DCV.
</commit_message>
<xml_diff>
--- a/tabular/contributed/190408 EBR TABLE.xlsx
+++ b/tabular/contributed/190408 EBR TABLE.xlsx
@@ -621,9 +621,6 @@
     <t>28I+30R+31M</t>
   </si>
   <si>
-    <t>HEPATHER</t>
-  </si>
-  <si>
     <t>EBR/GZR/RBV; EBR/GZR</t>
   </si>
   <si>
@@ -637,6 +634,9 @@
   </si>
   <si>
     <t>EBR/GZR/SOF</t>
+  </si>
+  <si>
+    <t>Real world (France)*</t>
   </si>
 </sst>
 </file>
@@ -1181,15 +1181,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="9"/>
-    <col min="2" max="2" width="12.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="9"/>
     <col min="3" max="3" width="23.6640625" style="9" customWidth="1"/>
     <col min="4" max="4" width="12" style="9" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="9" customWidth="1"/>
@@ -1210,11 +1210,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>8</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>9</v>
@@ -1263,10 +1263,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>99</v>
@@ -1293,7 +1293,7 @@
         <v>180</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16" t="s">
@@ -1309,10 +1309,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>100</v>
@@ -1339,7 +1339,7 @@
         <v>180</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16" t="s">
@@ -1354,11 +1354,11 @@
       <c r="R3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>4</v>
+      <c r="A4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>101</v>
@@ -1385,7 +1385,7 @@
         <v>180</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L4" s="16"/>
       <c r="M4" s="16" t="s">
@@ -1400,11 +1400,11 @@
       <c r="R4" s="19"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>4</v>
+      <c r="A5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>102</v>
@@ -1431,7 +1431,7 @@
         <v>180</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L5" s="16"/>
       <c r="M5" s="16" t="s">
@@ -1446,11 +1446,11 @@
       <c r="R5" s="16"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>4</v>
+      <c r="A6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>102</v>
@@ -1477,7 +1477,7 @@
         <v>180</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L6" s="16"/>
       <c r="M6" s="16" t="s">
@@ -1492,11 +1492,11 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>103</v>
@@ -1523,7 +1523,7 @@
         <v>180</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="16" t="s">
@@ -1538,11 +1538,11 @@
       <c r="R7" s="16"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>4</v>
+      <c r="A8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>104</v>
@@ -1569,7 +1569,7 @@
         <v>180</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="16" t="s">
@@ -1584,11 +1584,11 @@
       <c r="R8" s="16"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>4</v>
+      <c r="A9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>102</v>
@@ -1615,7 +1615,7 @@
         <v>180</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16" t="s">
@@ -1631,10 +1631,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>105</v>
@@ -1661,7 +1661,7 @@
         <v>180</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="16" t="s">
@@ -1676,11 +1676,11 @@
       <c r="R10" s="16"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>4</v>
+      <c r="A11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>106</v>
@@ -1707,7 +1707,7 @@
         <v>180</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16" t="s">
@@ -1722,11 +1722,11 @@
       <c r="R11" s="16"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>4</v>
+      <c r="A12" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>107</v>
@@ -1753,7 +1753,7 @@
         <v>180</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="16" t="s">
@@ -1768,11 +1768,11 @@
       <c r="R12" s="16"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>4</v>
+      <c r="A13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>171</v>
@@ -1814,11 +1814,11 @@
       <c r="R13" s="16"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>4</v>
+      <c r="A14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>108</v>
@@ -1860,11 +1860,11 @@
       <c r="R14" s="16"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>4</v>
+      <c r="A15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>109</v>
@@ -1906,11 +1906,11 @@
       <c r="R15" s="16"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>4</v>
+      <c r="A16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>172</v>
@@ -1952,11 +1952,11 @@
       <c r="R16" s="16"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>4</v>
+      <c r="A17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>107</v>
@@ -1998,11 +1998,11 @@
       <c r="R17" s="16"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>4</v>
+      <c r="A18" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>110</v>
@@ -2044,11 +2044,11 @@
       <c r="R18" s="16"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>4</v>
+      <c r="A19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>106</v>
@@ -2090,11 +2090,11 @@
       <c r="R19" s="16"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>4</v>
+      <c r="A20" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>111</v>
@@ -2136,11 +2136,11 @@
       <c r="R20" s="16"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>4</v>
+      <c r="A21" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>112</v>
@@ -2182,11 +2182,11 @@
       <c r="R21" s="16"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>4</v>
+      <c r="A22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>113</v>
@@ -2228,11 +2228,11 @@
       <c r="R22" s="16"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>4</v>
+      <c r="A23" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>102</v>
@@ -2274,11 +2274,11 @@
       <c r="R23" s="16"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>4</v>
+      <c r="A24" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>114</v>
@@ -2320,11 +2320,11 @@
       <c r="R24" s="16"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>4</v>
+      <c r="A25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>115</v>
@@ -2366,11 +2366,11 @@
       <c r="R25" s="16"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>116</v>
@@ -2412,11 +2412,11 @@
       <c r="R26" s="16"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>111</v>
@@ -2458,11 +2458,11 @@
       <c r="R27" s="16"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>110</v>
@@ -2504,11 +2504,11 @@
       <c r="R28" s="16"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>113</v>
@@ -2551,10 +2551,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>117</v>
@@ -2597,10 +2597,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>111</v>
@@ -2643,10 +2643,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>113</v>
@@ -2688,11 +2688,11 @@
       <c r="R32" s="16"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>4</v>
+      <c r="A33" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>118</v>
@@ -2719,7 +2719,7 @@
         <v>181</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="16" t="s">
@@ -2735,10 +2735,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>112</v>
@@ -2765,7 +2765,7 @@
         <v>181</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="16" t="s">
@@ -2780,11 +2780,11 @@
       <c r="R34" s="16"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>4</v>
+      <c r="A35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>107</v>
@@ -2811,7 +2811,7 @@
         <v>181</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L35" s="17"/>
       <c r="M35" s="16" t="s">
@@ -2826,11 +2826,11 @@
       <c r="R35" s="16"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>106</v>
@@ -2857,7 +2857,7 @@
         <v>181</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L36" s="17"/>
       <c r="M36" s="16" t="s">
@@ -2872,11 +2872,11 @@
       <c r="R36" s="16"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>113</v>
@@ -2903,7 +2903,7 @@
         <v>181</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L37" s="17"/>
       <c r="M37" s="16" t="s">
@@ -2918,11 +2918,11 @@
       <c r="R37" s="16"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>4</v>
+      <c r="A38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>119</v>
@@ -2964,11 +2964,11 @@
       <c r="R38" s="16"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>4</v>
+      <c r="A39" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>120</v>
@@ -3010,11 +3010,11 @@
       <c r="R39" s="16"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>4</v>
+      <c r="A40" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>121</v>
@@ -3056,11 +3056,11 @@
       <c r="R40" s="16"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>4</v>
+      <c r="A41" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>122</v>
@@ -3102,11 +3102,11 @@
       <c r="R41" s="16"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>4</v>
+      <c r="A42" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>107</v>
@@ -3148,11 +3148,11 @@
       <c r="R42" s="16"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>4</v>
+      <c r="A43" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>106</v>
@@ -3194,11 +3194,11 @@
       <c r="R43" s="16"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>4</v>
+      <c r="A44" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>110</v>
@@ -3240,11 +3240,11 @@
       <c r="R44" s="16"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>4</v>
+      <c r="A45" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>114</v>
@@ -3286,11 +3286,11 @@
       <c r="R45" s="16"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>4</v>
+      <c r="A46" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>113</v>
@@ -3332,11 +3332,11 @@
       <c r="R46" s="16"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A47" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>4</v>
+      <c r="A47" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>102</v>
@@ -3378,11 +3378,11 @@
       <c r="R47" s="16"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>4</v>
+      <c r="A48" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>123</v>
@@ -3424,11 +3424,11 @@
       <c r="R48" s="16"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>4</v>
+      <c r="A49" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>124</v>
@@ -3470,11 +3470,11 @@
       <c r="R49" s="16"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>4</v>
+      <c r="A50" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>125</v>
@@ -3516,11 +3516,11 @@
       <c r="R50" s="16"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>4</v>
+      <c r="A51" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>126</v>
@@ -3562,11 +3562,11 @@
       <c r="R51" s="16"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>4</v>
+      <c r="A52" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>127</v>
@@ -3608,11 +3608,11 @@
       <c r="R52" s="16"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>4</v>
+      <c r="A53" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>128</v>
@@ -3654,11 +3654,11 @@
       <c r="R53" s="16"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>4</v>
+      <c r="A54" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>129</v>
@@ -3700,11 +3700,11 @@
       <c r="R54" s="16"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>4</v>
+      <c r="A55" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>130</v>
@@ -3746,11 +3746,11 @@
       <c r="R55" s="16"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>4</v>
+      <c r="A56" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>131</v>
@@ -3792,11 +3792,11 @@
       <c r="R56" s="16"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>4</v>
+      <c r="A57" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>132</v>
@@ -3838,11 +3838,11 @@
       <c r="R57" s="16"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>4</v>
+      <c r="A58" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>133</v>
@@ -3884,11 +3884,11 @@
       <c r="R58" s="16"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>4</v>
+      <c r="A59" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>134</v>
@@ -3930,11 +3930,11 @@
       <c r="R59" s="16"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>4</v>
+      <c r="A60" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>99</v>
@@ -3961,7 +3961,7 @@
         <v>186</v>
       </c>
       <c r="K60" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L60" s="16"/>
       <c r="M60" s="16" t="s">
@@ -3976,11 +3976,11 @@
       <c r="R60" s="16"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>4</v>
+      <c r="A61" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>99</v>
@@ -4022,11 +4022,11 @@
       <c r="R61" s="16"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A62" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>4</v>
+      <c r="A62" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C62" s="16" t="s">
         <v>122</v>
@@ -4053,7 +4053,7 @@
         <v>186</v>
       </c>
       <c r="K62" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L62" s="16"/>
       <c r="M62" s="16" t="s">
@@ -4068,11 +4068,11 @@
       <c r="R62" s="16"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>4</v>
+      <c r="A63" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C63" s="16" t="s">
         <v>122</v>
@@ -4114,11 +4114,11 @@
       <c r="R63" s="16"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>4</v>
+      <c r="A64" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>135</v>
@@ -4145,7 +4145,7 @@
         <v>186</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L64" s="16"/>
       <c r="M64" s="16" t="s">
@@ -4160,11 +4160,11 @@
       <c r="R64" s="16"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A65" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>4</v>
+      <c r="A65" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>107</v>
@@ -4191,7 +4191,7 @@
         <v>186</v>
       </c>
       <c r="K65" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L65" s="16"/>
       <c r="M65" s="16" t="s">
@@ -4206,11 +4206,11 @@
       <c r="R65" s="16"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>4</v>
+      <c r="A66" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>107</v>
@@ -4252,11 +4252,11 @@
       <c r="R66" s="16"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>4</v>
+      <c r="A67" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>106</v>
@@ -4283,7 +4283,7 @@
         <v>186</v>
       </c>
       <c r="K67" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L67" s="16"/>
       <c r="M67" s="16" t="s">
@@ -4298,11 +4298,11 @@
       <c r="R67" s="16"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A68" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>4</v>
+      <c r="A68" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>106</v>
@@ -4344,11 +4344,11 @@
       <c r="R68" s="16"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>4</v>
+      <c r="A69" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>112</v>
@@ -4375,7 +4375,7 @@
         <v>186</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L69" s="16"/>
       <c r="M69" s="16" t="s">
@@ -4390,11 +4390,11 @@
       <c r="R69" s="16"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>4</v>
+      <c r="A70" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C70" s="16" t="s">
         <v>112</v>
@@ -4436,11 +4436,11 @@
       <c r="R70" s="16"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A71" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>4</v>
+      <c r="A71" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C71" s="16" t="s">
         <v>114</v>
@@ -4482,11 +4482,11 @@
       <c r="R71" s="16"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>4</v>
+      <c r="A72" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C72" s="16" t="s">
         <v>102</v>
@@ -4528,11 +4528,11 @@
       <c r="R72" s="16"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A73" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>4</v>
+      <c r="A73" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C73" s="16" t="s">
         <v>136</v>
@@ -4559,7 +4559,7 @@
         <v>186</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L73" s="16"/>
       <c r="M73" s="16" t="s">
@@ -4574,11 +4574,11 @@
       <c r="R73" s="16"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A74" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>4</v>
+      <c r="A74" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C74" s="16" t="s">
         <v>107</v>
@@ -4605,7 +4605,7 @@
         <v>182</v>
       </c>
       <c r="K74" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L74" s="16"/>
       <c r="M74" s="16" t="s">
@@ -4620,11 +4620,11 @@
       <c r="R74" s="16"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A75" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>4</v>
+      <c r="A75" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C75" s="16" t="s">
         <v>117</v>
@@ -4651,7 +4651,7 @@
         <v>182</v>
       </c>
       <c r="K75" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L75" s="16"/>
       <c r="M75" s="16" t="s">
@@ -4666,11 +4666,11 @@
       <c r="R75" s="16"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A76" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B76" s="17" t="s">
+      <c r="A76" s="17" t="s">
         <v>59</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C76" s="16" t="s">
         <v>48</v>
@@ -4697,7 +4697,7 @@
         <v>182</v>
       </c>
       <c r="K76" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L76" s="16"/>
       <c r="M76" s="16" t="s">
@@ -4712,11 +4712,11 @@
       <c r="R76" s="16"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A77" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>4</v>
+      <c r="A77" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C77" s="16" t="s">
         <v>102</v>
@@ -4743,7 +4743,7 @@
         <v>183</v>
       </c>
       <c r="K77" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L77" s="16"/>
       <c r="M77" s="16" t="s">
@@ -4758,11 +4758,11 @@
       <c r="R77" s="16"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A78" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>4</v>
+      <c r="A78" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>107</v>
@@ -4789,7 +4789,7 @@
         <v>183</v>
       </c>
       <c r="K78" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L78" s="16"/>
       <c r="M78" s="16" t="s">
@@ -4804,11 +4804,11 @@
       <c r="R78" s="16"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A79" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>4</v>
+      <c r="A79" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C79" s="16" t="s">
         <v>104</v>
@@ -4835,7 +4835,7 @@
         <v>183</v>
       </c>
       <c r="K79" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L79" s="16"/>
       <c r="M79" s="16" t="s">
@@ -4850,11 +4850,11 @@
       <c r="R79" s="16"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A80" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>4</v>
+      <c r="A80" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C80" s="16" t="s">
         <v>137</v>
@@ -4881,7 +4881,7 @@
         <v>183</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L80" s="16"/>
       <c r="M80" s="16" t="s">
@@ -4896,11 +4896,11 @@
       <c r="R80" s="16"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A81" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>4</v>
+      <c r="A81" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C81" s="16" t="s">
         <v>138</v>
@@ -4927,7 +4927,7 @@
         <v>183</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L81" s="16"/>
       <c r="M81" s="16" t="s">
@@ -4942,11 +4942,11 @@
       <c r="R81" s="16"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A82" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>4</v>
+      <c r="A82" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C82" s="16" t="s">
         <v>119</v>
@@ -4973,7 +4973,7 @@
         <v>183</v>
       </c>
       <c r="K82" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L82" s="16"/>
       <c r="M82" s="16" t="s">
@@ -4988,11 +4988,11 @@
       <c r="R82" s="16"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A83" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B83" s="17" t="s">
+      <c r="A83" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C83" s="16" t="s">
         <v>116</v>
@@ -5019,7 +5019,7 @@
         <v>183</v>
       </c>
       <c r="K83" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L83" s="16"/>
       <c r="M83" s="16" t="s">
@@ -5034,11 +5034,11 @@
       <c r="R83" s="16"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A84" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B84" s="17" t="s">
+      <c r="A84" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C84" s="16" t="s">
         <v>139</v>
@@ -5065,7 +5065,7 @@
         <v>183</v>
       </c>
       <c r="K84" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L84" s="16"/>
       <c r="M84" s="16" t="s">
@@ -5080,11 +5080,11 @@
       <c r="R84" s="16"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A85" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B85" s="17" t="s">
+      <c r="A85" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C85" s="16" t="s">
         <v>106</v>
@@ -5111,7 +5111,7 @@
         <v>183</v>
       </c>
       <c r="K85" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L85" s="16"/>
       <c r="M85" s="16" t="s">
@@ -5127,10 +5127,10 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C86" s="16" t="s">
         <v>113</v>
@@ -5157,7 +5157,7 @@
         <v>183</v>
       </c>
       <c r="K86" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L86" s="16"/>
       <c r="M86" s="16" t="s">
@@ -5173,10 +5173,10 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>113</v>
@@ -5203,7 +5203,7 @@
         <v>55</v>
       </c>
       <c r="K87" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L87" s="16"/>
       <c r="M87" s="16" t="s">
@@ -5218,11 +5218,11 @@
       <c r="R87" s="16"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A88" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B88" s="17" t="s">
+      <c r="A88" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C88" s="16" t="s">
         <v>106</v>
@@ -5249,7 +5249,7 @@
         <v>55</v>
       </c>
       <c r="K88" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L88" s="16"/>
       <c r="M88" s="16" t="s">
@@ -5264,11 +5264,11 @@
       <c r="R88" s="16"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A89" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B89" s="17" t="s">
+      <c r="A89" s="17" t="s">
         <v>3</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>106</v>
@@ -5295,7 +5295,7 @@
         <v>55</v>
       </c>
       <c r="K89" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L89" s="16"/>
       <c r="M89" s="16" t="s">
@@ -5311,10 +5311,10 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>103</v>
@@ -5341,7 +5341,7 @@
         <v>55</v>
       </c>
       <c r="K90" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L90" s="16"/>
       <c r="M90" s="16" t="s">
@@ -5357,10 +5357,10 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C91" s="16" t="s">
         <v>140</v>
@@ -5387,7 +5387,7 @@
         <v>187</v>
       </c>
       <c r="K91" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L91" s="16"/>
       <c r="M91" s="16" t="s">
@@ -5402,11 +5402,11 @@
       <c r="R91" s="16"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A92" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>4</v>
+      <c r="A92" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C92" s="16" t="s">
         <v>106</v>
@@ -5433,7 +5433,7 @@
         <v>187</v>
       </c>
       <c r="K92" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L92" s="29"/>
       <c r="M92" s="16" t="s">
@@ -5448,11 +5448,11 @@
       <c r="R92" s="16"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A93" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B93" s="17" t="s">
-        <v>4</v>
+      <c r="A93" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C93" s="16" t="s">
         <v>107</v>
@@ -5479,7 +5479,7 @@
         <v>187</v>
       </c>
       <c r="K93" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L93" s="16"/>
       <c r="M93" s="16" t="s">
@@ -5494,11 +5494,11 @@
       <c r="R93" s="16"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A94" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>4</v>
+      <c r="A94" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C94" s="16" t="s">
         <v>141</v>
@@ -5525,7 +5525,7 @@
         <v>187</v>
       </c>
       <c r="K94" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L94" s="16"/>
       <c r="M94" s="16" t="s">
@@ -5540,11 +5540,11 @@
       <c r="R94" s="16"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A95" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B95" s="17" t="s">
-        <v>4</v>
+      <c r="A95" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C95" s="16" t="s">
         <v>122</v>
@@ -5571,7 +5571,7 @@
         <v>187</v>
       </c>
       <c r="K95" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L95" s="17"/>
       <c r="M95" s="16" t="s">
@@ -5586,11 +5586,11 @@
       <c r="R95" s="16"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A96" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>4</v>
+      <c r="A96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C96" s="16" t="s">
         <v>112</v>
@@ -5617,7 +5617,7 @@
         <v>187</v>
       </c>
       <c r="K96" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L96" s="16"/>
       <c r="M96" s="16" t="s">
@@ -5632,11 +5632,11 @@
       <c r="R96" s="16"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A97" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B97" s="17" t="s">
-        <v>4</v>
+      <c r="A97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C97" s="16" t="s">
         <v>142</v>
@@ -5663,7 +5663,7 @@
         <v>187</v>
       </c>
       <c r="K97" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L97" s="16"/>
       <c r="M97" s="16" t="s">
@@ -5678,11 +5678,11 @@
       <c r="R97" s="16"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A98" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="17" t="s">
-        <v>4</v>
+      <c r="A98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C98" s="16" t="s">
         <v>106</v>
@@ -5709,7 +5709,7 @@
         <v>187</v>
       </c>
       <c r="K98" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L98" s="16"/>
       <c r="M98" s="16" t="s">
@@ -5724,11 +5724,11 @@
       <c r="R98" s="16"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A99" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B99" s="17" t="s">
-        <v>4</v>
+      <c r="A99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C99" s="16" t="s">
         <v>127</v>
@@ -5755,7 +5755,7 @@
         <v>187</v>
       </c>
       <c r="K99" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L99" s="16"/>
       <c r="M99" s="16" t="s">
@@ -5770,11 +5770,11 @@
       <c r="R99" s="16"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A100" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B100" s="17" t="s">
-        <v>4</v>
+      <c r="A100" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C100" s="16" t="s">
         <v>107</v>
@@ -5801,7 +5801,7 @@
         <v>187</v>
       </c>
       <c r="K100" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L100" s="16"/>
       <c r="M100" s="16" t="s">
@@ -5816,11 +5816,11 @@
       <c r="R100" s="16"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A101" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B101" s="17" t="s">
-        <v>4</v>
+      <c r="A101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C101" s="16" t="s">
         <v>102</v>
@@ -5847,7 +5847,7 @@
         <v>187</v>
       </c>
       <c r="K101" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L101" s="16"/>
       <c r="M101" s="16" t="s">
@@ -5863,10 +5863,10 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C102" s="16" t="s">
         <v>113</v>
@@ -5893,7 +5893,7 @@
         <v>187</v>
       </c>
       <c r="K102" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L102" s="16"/>
       <c r="M102" s="16" t="s">
@@ -5909,10 +5909,10 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C103" s="16" t="s">
         <v>106</v>
@@ -5939,7 +5939,7 @@
         <v>187</v>
       </c>
       <c r="K103" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L103" s="16"/>
       <c r="M103" s="16" t="s">
@@ -5955,10 +5955,10 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="16" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C104" s="16" t="s">
         <v>143</v>
@@ -5985,7 +5985,7 @@
         <v>187</v>
       </c>
       <c r="K104" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L104" s="16"/>
       <c r="M104" s="16" t="s">
@@ -6001,10 +6001,10 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" s="16" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C105" s="16" t="s">
         <v>144</v>
@@ -6031,7 +6031,7 @@
         <v>187</v>
       </c>
       <c r="K105" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L105" s="16"/>
       <c r="M105" s="16" t="s">
@@ -6047,10 +6047,10 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" s="16" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C106" s="16" t="s">
         <v>126</v>
@@ -6077,7 +6077,7 @@
         <v>187</v>
       </c>
       <c r="K106" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L106" s="16"/>
       <c r="M106" s="16" t="s">
@@ -6093,10 +6093,10 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" s="16" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C107" s="16" t="s">
         <v>145</v>
@@ -6123,7 +6123,7 @@
         <v>187</v>
       </c>
       <c r="K107" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L107" s="16"/>
       <c r="M107" s="16" t="s">
@@ -6139,10 +6139,10 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" s="16" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C108" s="16" t="s">
         <v>112</v>
@@ -6169,7 +6169,7 @@
         <v>187</v>
       </c>
       <c r="K108" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L108" s="16"/>
       <c r="M108" s="16" t="s">
@@ -6185,10 +6185,10 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C109" s="16" t="s">
         <v>142</v>
@@ -6215,7 +6215,7 @@
         <v>57</v>
       </c>
       <c r="K109" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L109" s="16"/>
       <c r="M109" s="16" t="s">
@@ -6230,11 +6230,11 @@
       <c r="R109" s="16"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A110" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B110" s="20" t="s">
-        <v>4</v>
+      <c r="A110" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C110" s="20" t="s">
         <v>106</v>
@@ -6261,7 +6261,7 @@
         <v>57</v>
       </c>
       <c r="K110" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L110" s="20"/>
       <c r="M110" s="16" t="s">
@@ -6276,11 +6276,11 @@
       <c r="R110" s="20"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A111" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B111" s="20" t="s">
-        <v>4</v>
+      <c r="A111" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C111" s="20" t="s">
         <v>127</v>
@@ -6307,7 +6307,7 @@
         <v>57</v>
       </c>
       <c r="K111" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L111" s="20"/>
       <c r="M111" s="16" t="s">
@@ -6323,10 +6323,10 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C112" s="20" t="s">
         <v>146</v>
@@ -6353,7 +6353,7 @@
         <v>57</v>
       </c>
       <c r="K112" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L112" s="20"/>
       <c r="M112" s="16" t="s">
@@ -6369,10 +6369,10 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C113" s="20" t="s">
         <v>147</v>
@@ -6399,7 +6399,7 @@
         <v>57</v>
       </c>
       <c r="K113" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L113" s="20"/>
       <c r="M113" s="16" t="s">
@@ -6415,10 +6415,10 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C114" s="20" t="s">
         <v>148</v>
@@ -6445,7 +6445,7 @@
         <v>57</v>
       </c>
       <c r="K114" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L114" s="20"/>
       <c r="M114" s="16" t="s">
@@ -6461,10 +6461,10 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C115" s="20" t="s">
         <v>149</v>
@@ -6491,7 +6491,7 @@
         <v>57</v>
       </c>
       <c r="K115" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L115" s="20"/>
       <c r="M115" s="16" t="s">
@@ -6507,10 +6507,10 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C116" s="20" t="s">
         <v>106</v>
@@ -6537,7 +6537,7 @@
         <v>57</v>
       </c>
       <c r="K116" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L116" s="20"/>
       <c r="M116" s="16" t="s">
@@ -6552,11 +6552,11 @@
       <c r="R116" s="20"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A117" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B117" s="20" t="s">
-        <v>4</v>
+      <c r="A117" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C117" s="20" t="s">
         <v>107</v>
@@ -6583,7 +6583,7 @@
         <v>57</v>
       </c>
       <c r="K117" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L117" s="20"/>
       <c r="M117" s="16" t="s">
@@ -6599,10 +6599,10 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C118" s="20" t="s">
         <v>113</v>
@@ -6629,7 +6629,7 @@
         <v>57</v>
       </c>
       <c r="K118" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L118" s="20"/>
       <c r="M118" s="16" t="s">
@@ -6645,10 +6645,10 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C119" s="20" t="s">
         <v>106</v>
@@ -6675,7 +6675,7 @@
         <v>57</v>
       </c>
       <c r="K119" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L119" s="20"/>
       <c r="M119" s="16" t="s">
@@ -6690,11 +6690,11 @@
       <c r="R119" s="20"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A120" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B120" s="20">
-        <v>4</v>
+      <c r="A120" s="20">
+        <v>4</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C120" s="30" t="s">
         <v>150</v>
@@ -6736,11 +6736,11 @@
       <c r="R120" s="30"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A121" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B121" s="20">
-        <v>4</v>
+      <c r="A121" s="20">
+        <v>4</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C121" s="30" t="s">
         <v>151</v>
@@ -6782,11 +6782,11 @@
       <c r="R121" s="30"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A122" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B122" s="20">
-        <v>4</v>
+      <c r="A122" s="20">
+        <v>4</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C122" s="30" t="s">
         <v>173</v>
@@ -6828,11 +6828,11 @@
       <c r="R122" s="30"/>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A123" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B123" s="30">
-        <v>4</v>
+      <c r="A123" s="30">
+        <v>4</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C123" s="30" t="s">
         <v>113</v>
@@ -6874,11 +6874,11 @@
       <c r="R123" s="30"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A124" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B124" s="20" t="s">
-        <v>4</v>
+      <c r="A124" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C124" s="30" t="s">
         <v>119</v>
@@ -6905,7 +6905,7 @@
         <v>70</v>
       </c>
       <c r="K124" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L124" s="20"/>
       <c r="M124" s="16" t="s">
@@ -6920,11 +6920,11 @@
       <c r="R124" s="30"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A125" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B125" s="20" t="s">
-        <v>4</v>
+      <c r="A125" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C125" s="30" t="s">
         <v>48</v>
@@ -6951,7 +6951,7 @@
         <v>70</v>
       </c>
       <c r="K125" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L125" s="20"/>
       <c r="M125" s="16" t="s">
@@ -6966,11 +6966,11 @@
       <c r="R125" s="30"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A126" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B126" s="20" t="s">
-        <v>4</v>
+      <c r="A126" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C126" s="30" t="s">
         <v>113</v>
@@ -6997,7 +6997,7 @@
         <v>70</v>
       </c>
       <c r="K126" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L126" s="20"/>
       <c r="M126" s="16" t="s">
@@ -7012,11 +7012,11 @@
       <c r="R126" s="30"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A127" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B127" s="30" t="s">
-        <v>4</v>
+      <c r="A127" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C127" s="30" t="s">
         <v>102</v>
@@ -7043,7 +7043,7 @@
         <v>70</v>
       </c>
       <c r="K127" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L127" s="20"/>
       <c r="M127" s="16" t="s">
@@ -7058,11 +7058,11 @@
       <c r="R127" s="30"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A128" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B128" s="30" t="s">
+      <c r="A128" s="30" t="s">
         <v>3</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C128" s="30" t="s">
         <v>106</v>
@@ -7089,7 +7089,7 @@
         <v>70</v>
       </c>
       <c r="K128" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L128" s="20"/>
       <c r="M128" s="16" t="s">
@@ -7104,11 +7104,11 @@
       <c r="R128" s="30"/>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A129" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B129" s="20">
+      <c r="A129" s="20">
         <v>3</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C129" s="30" t="s">
         <v>135</v>
@@ -7135,7 +7135,7 @@
         <v>73</v>
       </c>
       <c r="K129" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L129" s="20"/>
       <c r="M129" s="16" t="s">
@@ -7150,11 +7150,11 @@
       <c r="R129" s="30"/>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A130" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B130" s="20">
+      <c r="A130" s="20">
         <v>3</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C130" s="30" t="s">
         <v>152</v>
@@ -7181,7 +7181,7 @@
         <v>73</v>
       </c>
       <c r="K130" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L130" s="20"/>
       <c r="M130" s="16" t="s">
@@ -7196,11 +7196,11 @@
       <c r="R130" s="30"/>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A131" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B131" s="20">
+      <c r="A131" s="20">
         <v>3</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C131" s="30" t="s">
         <v>153</v>
@@ -7227,7 +7227,7 @@
         <v>73</v>
       </c>
       <c r="K131" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L131" s="20"/>
       <c r="M131" s="16" t="s">
@@ -7242,11 +7242,11 @@
       <c r="R131" s="30"/>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A132" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B132" s="20">
+      <c r="A132" s="20">
         <v>3</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C132" s="30" t="s">
         <v>113</v>
@@ -7273,7 +7273,7 @@
         <v>73</v>
       </c>
       <c r="K132" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L132" s="20"/>
       <c r="M132" s="16" t="s">
@@ -7288,11 +7288,11 @@
       <c r="R132" s="30"/>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A133" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B133" s="20">
+      <c r="A133" s="20">
         <v>3</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C133" s="30" t="s">
         <v>154</v>
@@ -7319,7 +7319,7 @@
         <v>73</v>
       </c>
       <c r="K133" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L133" s="20"/>
       <c r="M133" s="16" t="s">
@@ -7334,11 +7334,11 @@
       <c r="R133" s="30"/>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A134" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B134" s="20">
+      <c r="A134" s="20">
         <v>3</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C134" s="30" t="s">
         <v>111</v>
@@ -7365,7 +7365,7 @@
         <v>73</v>
       </c>
       <c r="K134" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L134" s="20"/>
       <c r="M134" s="16" t="s">
@@ -7380,11 +7380,11 @@
       <c r="R134" s="30"/>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A135" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B135" s="20">
+      <c r="A135" s="20">
         <v>3</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C135" s="30" t="s">
         <v>117</v>
@@ -7411,7 +7411,7 @@
         <v>73</v>
       </c>
       <c r="K135" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L135" s="20"/>
       <c r="M135" s="16" t="s">
@@ -7426,11 +7426,11 @@
       <c r="R135" s="30"/>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A136" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B136" s="20">
+      <c r="A136" s="20">
         <v>3</v>
+      </c>
+      <c r="B136" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C136" s="30" t="s">
         <v>155</v>
@@ -7457,7 +7457,7 @@
         <v>73</v>
       </c>
       <c r="K136" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L136" s="20"/>
       <c r="M136" s="16" t="s">
@@ -7472,11 +7472,11 @@
       <c r="R136" s="30"/>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A137" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B137" s="20" t="s">
+      <c r="A137" s="20" t="s">
         <v>6</v>
+      </c>
+      <c r="B137" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C137" s="30" t="s">
         <v>156</v>
@@ -7518,11 +7518,11 @@
       <c r="R137" s="30"/>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A138" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B138" s="20" t="s">
+      <c r="A138" s="20" t="s">
         <v>6</v>
+      </c>
+      <c r="B138" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C138" s="30" t="s">
         <v>154</v>
@@ -7564,11 +7564,11 @@
       <c r="R138" s="30"/>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A139" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B139" s="20" t="s">
+      <c r="A139" s="20" t="s">
         <v>6</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C139" s="20" t="s">
         <v>177</v>
@@ -7610,11 +7610,11 @@
       <c r="R139" s="20"/>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A140" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B140" s="30" t="s">
-        <v>4</v>
+      <c r="A140" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B140" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C140" s="30" t="s">
         <v>122</v>
@@ -7656,11 +7656,11 @@
       <c r="R140" s="30"/>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A141" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B141" s="30" t="s">
-        <v>4</v>
+      <c r="A141" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B141" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C141" s="30" t="s">
         <v>107</v>
@@ -7702,11 +7702,11 @@
       <c r="R141" s="30"/>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A142" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B142" s="30" t="s">
-        <v>4</v>
+      <c r="A142" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C142" s="30" t="s">
         <v>117</v>
@@ -7748,11 +7748,11 @@
       <c r="R142" s="30"/>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A143" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B143" s="30" t="s">
-        <v>4</v>
+      <c r="A143" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C143" s="30" t="s">
         <v>113</v>
@@ -7794,11 +7794,11 @@
       <c r="R143" s="30"/>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A144" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B144" s="30" t="s">
-        <v>4</v>
+      <c r="A144" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B144" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C144" s="30" t="s">
         <v>114</v>
@@ -7840,11 +7840,11 @@
       <c r="R144" s="30"/>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A145" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B145" s="30" t="s">
-        <v>4</v>
+      <c r="A145" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C145" s="30" t="s">
         <v>102</v>
@@ -7886,11 +7886,11 @@
       <c r="R145" s="30"/>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A146" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B146" s="30" t="s">
-        <v>4</v>
+      <c r="A146" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C146" s="30" t="s">
         <v>110</v>
@@ -7932,11 +7932,11 @@
       <c r="R146" s="30"/>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A147" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B147" s="30" t="s">
-        <v>4</v>
+      <c r="A147" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C147" s="30" t="s">
         <v>174</v>
@@ -7978,11 +7978,11 @@
       <c r="R147" s="30"/>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A148" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B148" s="30" t="s">
+      <c r="A148" s="30" t="s">
         <v>3</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C148" s="30" t="s">
         <v>113</v>
@@ -8024,11 +8024,11 @@
       <c r="R148" s="30"/>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A149" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B149" s="30" t="s">
+      <c r="A149" s="30" t="s">
         <v>3</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C149" s="30" t="s">
         <v>102</v>
@@ -8070,11 +8070,11 @@
       <c r="R149" s="30"/>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A150" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B150" s="30" t="s">
+      <c r="A150" s="30" t="s">
         <v>3</v>
+      </c>
+      <c r="B150" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C150" s="30" t="s">
         <v>157</v>
@@ -8116,11 +8116,11 @@
       <c r="R150" s="30"/>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A151" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B151" s="30" t="s">
+      <c r="A151" s="30" t="s">
         <v>3</v>
+      </c>
+      <c r="B151" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C151" s="30" t="s">
         <v>174</v>
@@ -8162,11 +8162,11 @@
       <c r="R151" s="30"/>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A152" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B152" s="30" t="s">
+      <c r="A152" s="30" t="s">
         <v>3</v>
+      </c>
+      <c r="B152" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C152" s="30" t="s">
         <v>103</v>
@@ -8208,11 +8208,11 @@
       <c r="R152" s="30"/>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A153" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B153" s="30" t="s">
+      <c r="A153" s="30" t="s">
         <v>76</v>
+      </c>
+      <c r="B153" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C153" s="30" t="s">
         <v>48</v>
@@ -8254,11 +8254,11 @@
       <c r="R153" s="30"/>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A154" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B154" s="30" t="s">
+      <c r="A154" s="30" t="s">
         <v>76</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C154" s="30" t="s">
         <v>113</v>
@@ -8300,11 +8300,11 @@
       <c r="R154" s="30"/>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A155" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B155" s="30" t="s">
+      <c r="A155" s="30" t="s">
         <v>76</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C155" s="30" t="s">
         <v>158</v>
@@ -8346,11 +8346,11 @@
       <c r="R155" s="30"/>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A156" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B156" s="30" t="s">
+      <c r="A156" s="30" t="s">
         <v>76</v>
+      </c>
+      <c r="B156" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C156" s="30" t="s">
         <v>159</v>
@@ -8392,11 +8392,11 @@
       <c r="R156" s="30"/>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A157" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B157" s="30" t="s">
+      <c r="A157" s="30" t="s">
         <v>76</v>
+      </c>
+      <c r="B157" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C157" s="30" t="s">
         <v>110</v>
@@ -8438,11 +8438,11 @@
       <c r="R157" s="30"/>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A158" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B158" s="30" t="s">
+      <c r="A158" s="30" t="s">
         <v>76</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C158" s="30" t="s">
         <v>106</v>
@@ -8484,11 +8484,11 @@
       <c r="R158" s="30"/>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A159" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B159" s="30" t="s">
+      <c r="A159" s="30" t="s">
         <v>78</v>
+      </c>
+      <c r="B159" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C159" s="30" t="s">
         <v>113</v>
@@ -8530,11 +8530,11 @@
       <c r="R159" s="30"/>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A160" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B160" s="30" t="s">
+      <c r="A160" s="30" t="s">
         <v>78</v>
+      </c>
+      <c r="B160" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C160" s="30" t="s">
         <v>160</v>
@@ -8576,11 +8576,11 @@
       <c r="R160" s="30"/>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A161" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B161" s="30" t="s">
+      <c r="A161" s="30" t="s">
         <v>78</v>
+      </c>
+      <c r="B161" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C161" s="30" t="s">
         <v>161</v>
@@ -8622,11 +8622,11 @@
       <c r="R161" s="30"/>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A162" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B162" s="30" t="s">
+      <c r="A162" s="30" t="s">
         <v>6</v>
+      </c>
+      <c r="B162" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C162" s="30" t="s">
         <v>111</v>
@@ -8668,11 +8668,11 @@
       <c r="R162" s="30"/>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A163" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B163" s="30" t="s">
+      <c r="A163" s="30" t="s">
         <v>6</v>
+      </c>
+      <c r="B163" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C163" s="30" t="s">
         <v>113</v>
@@ -8714,11 +8714,11 @@
       <c r="R163" s="30"/>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A164" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B164" s="30" t="s">
+      <c r="A164" s="30" t="s">
         <v>6</v>
+      </c>
+      <c r="B164" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C164" s="30" t="s">
         <v>162</v>
@@ -8760,11 +8760,11 @@
       <c r="R164" s="30"/>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A165" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B165" s="30" t="s">
+      <c r="A165" s="30" t="s">
         <v>6</v>
+      </c>
+      <c r="B165" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C165" s="30" t="s">
         <v>163</v>
@@ -8806,11 +8806,11 @@
       <c r="R165" s="30"/>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A166" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B166" s="30" t="s">
+      <c r="A166" s="30" t="s">
         <v>6</v>
+      </c>
+      <c r="B166" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C166" s="30" t="s">
         <v>110</v>
@@ -8852,11 +8852,11 @@
       <c r="R166" s="30"/>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A167" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B167" s="30" t="s">
+      <c r="A167" s="30" t="s">
         <v>61</v>
+      </c>
+      <c r="B167" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C167" s="30" t="s">
         <v>122</v>
@@ -8898,11 +8898,11 @@
       <c r="R167" s="30"/>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A168" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B168" s="30" t="s">
+      <c r="A168" s="30" t="s">
         <v>61</v>
+      </c>
+      <c r="B168" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C168" s="30" t="s">
         <v>164</v>
@@ -8944,11 +8944,11 @@
       <c r="R168" s="30"/>
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A169" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B169" s="30" t="s">
+      <c r="A169" s="30" t="s">
         <v>79</v>
+      </c>
+      <c r="B169" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C169" s="30" t="s">
         <v>111</v>
@@ -8990,11 +8990,11 @@
       <c r="R169" s="30"/>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A170" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B170" s="30" t="s">
+      <c r="A170" s="30" t="s">
         <v>79</v>
+      </c>
+      <c r="B170" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C170" s="30" t="s">
         <v>110</v>
@@ -9036,11 +9036,11 @@
       <c r="R170" s="30"/>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A171" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B171" s="30" t="s">
+      <c r="A171" s="30" t="s">
         <v>79</v>
+      </c>
+      <c r="B171" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C171" s="20" t="s">
         <v>165</v>
@@ -9082,11 +9082,11 @@
       <c r="R171" s="20"/>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A172" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B172" s="30" t="s">
+      <c r="A172" s="30" t="s">
         <v>80</v>
+      </c>
+      <c r="B172" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C172" s="30" t="s">
         <v>110</v>
@@ -9128,11 +9128,11 @@
       <c r="R172" s="30"/>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A173" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B173" s="30" t="s">
+      <c r="A173" s="30" t="s">
         <v>80</v>
+      </c>
+      <c r="B173" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C173" s="30" t="s">
         <v>106</v>
@@ -9174,11 +9174,11 @@
       <c r="R173" s="30"/>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A174" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B174" s="30" t="s">
+      <c r="A174" s="30" t="s">
         <v>81</v>
+      </c>
+      <c r="B174" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C174" s="30" t="s">
         <v>111</v>
@@ -9220,11 +9220,11 @@
       <c r="R174" s="30"/>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A175" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B175" s="30" t="s">
+      <c r="A175" s="30" t="s">
         <v>81</v>
+      </c>
+      <c r="B175" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C175" s="20" t="s">
         <v>175</v>
@@ -9266,11 +9266,11 @@
       <c r="R175" s="20"/>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A176" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B176" s="30" t="s">
+      <c r="A176" s="30" t="s">
         <v>81</v>
+      </c>
+      <c r="B176" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="C176" s="20" t="s">
         <v>176</v>
@@ -9312,11 +9312,11 @@
       <c r="R176" s="20"/>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A177" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B177" s="26">
+      <c r="A177" s="26">
         <v>3</v>
+      </c>
+      <c r="B177" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="C177" s="32" t="s">
         <v>166</v>
@@ -9343,7 +9343,7 @@
         <v>184</v>
       </c>
       <c r="K177" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L177" s="11"/>
       <c r="M177" s="26" t="s">
@@ -9358,11 +9358,11 @@
       <c r="R177" s="32"/>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A178" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B178" s="20">
-        <v>4</v>
+      <c r="A178" s="20">
+        <v>4</v>
+      </c>
+      <c r="B178" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="C178" s="30" t="s">
         <v>167</v>
@@ -9389,7 +9389,7 @@
         <v>84</v>
       </c>
       <c r="K178" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L178" s="11"/>
       <c r="M178" s="20" t="s">
@@ -9404,11 +9404,11 @@
       <c r="R178" s="30"/>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A179" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B179" s="20">
-        <v>4</v>
+      <c r="A179" s="20">
+        <v>4</v>
+      </c>
+      <c r="B179" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="C179" s="30" t="s">
         <v>143</v>
@@ -9435,7 +9435,7 @@
         <v>84</v>
       </c>
       <c r="K179" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L179" s="11"/>
       <c r="M179" s="20" t="s">
@@ -9451,10 +9451,10 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" s="20" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B180" s="20" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C180" s="30" t="s">
         <v>168</v>
@@ -9481,7 +9481,7 @@
         <v>188</v>
       </c>
       <c r="K180" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L180" s="11"/>
       <c r="M180" s="20" t="s">
@@ -9497,10 +9497,10 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" s="26" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C181" s="32" t="s">
         <v>119</v>
@@ -9527,7 +9527,7 @@
         <v>188</v>
       </c>
       <c r="K181" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L181" s="11"/>
       <c r="M181" s="26" t="s">
@@ -9543,10 +9543,10 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" s="20" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B182" s="20" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="C182" s="30" t="s">
         <v>169</v>
@@ -9573,7 +9573,7 @@
         <v>188</v>
       </c>
       <c r="K182" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L182" s="11"/>
       <c r="M182" s="30" t="s">
@@ -9589,10 +9589,10 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" s="20" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B183" s="20" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="C183" s="20" t="s">
         <v>114</v>
@@ -9619,7 +9619,7 @@
         <v>188</v>
       </c>
       <c r="K183" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L183" s="11"/>
       <c r="M183" s="30" t="s">
@@ -9634,11 +9634,11 @@
       <c r="R183" s="20"/>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A184" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B184" s="30" t="s">
-        <v>4</v>
+      <c r="A184" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C184" s="30" t="s">
         <v>99</v>
@@ -9665,7 +9665,7 @@
         <v>185</v>
       </c>
       <c r="K184" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L184" s="11"/>
       <c r="M184" s="30" t="s">
@@ -9680,11 +9680,11 @@
       <c r="R184" s="30"/>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A185" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B185" s="34" t="s">
-        <v>4</v>
+      <c r="A185" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C185" s="34" t="s">
         <v>122</v>
@@ -9726,11 +9726,11 @@
       <c r="R185" s="34"/>
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A186" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B186" s="34" t="s">
-        <v>4</v>
+      <c r="A186" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C186" s="34" t="s">
         <v>107</v>
@@ -9772,11 +9772,11 @@
       <c r="R186" s="34"/>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A187" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B187" s="34" t="s">
-        <v>4</v>
+      <c r="A187" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C187" s="34" t="s">
         <v>111</v>
@@ -9818,11 +9818,11 @@
       <c r="R187" s="34"/>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A188" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B188" s="34" t="s">
-        <v>4</v>
+      <c r="A188" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C188" s="34" t="s">
         <v>110</v>
@@ -9864,11 +9864,11 @@
       <c r="R188" s="34"/>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A189" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B189" s="34" t="s">
-        <v>4</v>
+      <c r="A189" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C189" s="34" t="s">
         <v>114</v>
@@ -9910,11 +9910,11 @@
       <c r="R189" s="34"/>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A190" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B190" s="34" t="s">
-        <v>4</v>
+      <c r="A190" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B190" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C190" s="34" t="s">
         <v>113</v>
@@ -9956,11 +9956,11 @@
       <c r="R190" s="34"/>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A191" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B191" s="34" t="s">
+      <c r="A191" s="34" t="s">
         <v>3</v>
+      </c>
+      <c r="B191" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C191" s="34" t="s">
         <v>170</v>
@@ -10002,11 +10002,11 @@
       <c r="R191" s="34"/>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A192" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B192" s="34" t="s">
+      <c r="A192" s="34" t="s">
         <v>3</v>
+      </c>
+      <c r="B192" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C192" s="34" t="s">
         <v>111</v>
@@ -10048,11 +10048,11 @@
       <c r="R192" s="34"/>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A193" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B193" s="34" t="s">
+      <c r="A193" s="34" t="s">
         <v>3</v>
+      </c>
+      <c r="B193" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C193" s="34" t="s">
         <v>110</v>
@@ -10094,11 +10094,11 @@
       <c r="R193" s="34"/>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A194" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B194" s="34" t="s">
+      <c r="A194" s="34" t="s">
         <v>3</v>
+      </c>
+      <c r="B194" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C194" s="34" t="s">
         <v>113</v>
@@ -10141,10 +10141,10 @@
     </row>
     <row r="195" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="40" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="B195" s="40" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C195" s="40" t="s">
         <v>196</v>
@@ -10163,17 +10163,17 @@
       </c>
       <c r="I195" s="41"/>
       <c r="J195" s="40" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="K195" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O195" s="40">
         <v>30125371</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P102">
+  <sortState ref="B2:Q102">
     <sortCondition ref="C2:C102"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working extension of resistance evidence base to grazoprevir.
</commit_message>
<xml_diff>
--- a/tabular/contributed/190408 EBR TABLE.xlsx
+++ b/tabular/contributed/190408 EBR TABLE.xlsx
@@ -600,18 +600,9 @@
     <t>C-EDGE TN</t>
   </si>
   <si>
-    <t>C‐SCAPE </t>
-  </si>
-  <si>
-    <t>C‐EDGE IBLD</t>
-  </si>
-  <si>
     <t>C-CORAL</t>
   </si>
   <si>
-    <t>C‐EDGE Head‐2‐head</t>
-  </si>
-  <si>
     <t>EBR</t>
   </si>
   <si>
@@ -637,6 +628,15 @@
   </si>
   <si>
     <t>Real world (France)*</t>
+  </si>
+  <si>
+    <t>C-SCAPE </t>
+  </si>
+  <si>
+    <t>C-EDGE IBLD</t>
+  </si>
+  <si>
+    <t>C-EDGE Head-2-head</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B196" sqref="B196"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1281,7 +1281,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>1</v>
@@ -1293,7 +1293,7 @@
         <v>180</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16" t="s">
@@ -1327,7 +1327,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>1</v>
@@ -1339,7 +1339,7 @@
         <v>180</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16" t="s">
@@ -1373,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>1</v>
@@ -1385,7 +1385,7 @@
         <v>180</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L4" s="16"/>
       <c r="M4" s="16" t="s">
@@ -1419,7 +1419,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>1</v>
@@ -1431,7 +1431,7 @@
         <v>180</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L5" s="16"/>
       <c r="M5" s="16" t="s">
@@ -1465,7 +1465,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>1</v>
@@ -1477,7 +1477,7 @@
         <v>180</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L6" s="16"/>
       <c r="M6" s="16" t="s">
@@ -1511,7 +1511,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>1</v>
@@ -1523,7 +1523,7 @@
         <v>180</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="16" t="s">
@@ -1557,7 +1557,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>1</v>
@@ -1569,7 +1569,7 @@
         <v>180</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="16" t="s">
@@ -1603,7 +1603,7 @@
         <v>30</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>1</v>
@@ -1615,7 +1615,7 @@
         <v>180</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16" t="s">
@@ -1649,7 +1649,7 @@
         <v>30</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>1</v>
@@ -1661,7 +1661,7 @@
         <v>180</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="16" t="s">
@@ -1695,7 +1695,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>1</v>
@@ -1707,7 +1707,7 @@
         <v>180</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16" t="s">
@@ -1741,7 +1741,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>1</v>
@@ -1753,7 +1753,7 @@
         <v>180</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="16" t="s">
@@ -1787,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>5</v>
@@ -1833,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>5</v>
@@ -1879,7 +1879,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>5</v>
@@ -1925,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>5</v>
@@ -1971,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>5</v>
@@ -2017,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>5</v>
@@ -2063,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H19" s="17" t="s">
         <v>5</v>
@@ -2109,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>5</v>
@@ -2155,7 +2155,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>5</v>
@@ -2201,7 +2201,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>5</v>
@@ -2247,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>5</v>
@@ -2293,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>5</v>
@@ -2339,7 +2339,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>5</v>
@@ -2385,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>5</v>
@@ -2431,7 +2431,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>5</v>
@@ -2477,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>5</v>
@@ -2523,7 +2523,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>5</v>
@@ -2569,7 +2569,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H30" s="24" t="s">
         <v>5</v>
@@ -2615,7 +2615,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H31" s="17" t="s">
         <v>5</v>
@@ -2661,7 +2661,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>5</v>
@@ -2707,7 +2707,7 @@
         <v>35</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>1</v>
@@ -2719,7 +2719,7 @@
         <v>181</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="16" t="s">
@@ -2753,7 +2753,7 @@
         <v>35</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H34" s="17" t="s">
         <v>1</v>
@@ -2765,7 +2765,7 @@
         <v>181</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="16" t="s">
@@ -2799,7 +2799,7 @@
         <v>31</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>1</v>
@@ -2811,7 +2811,7 @@
         <v>181</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L35" s="17"/>
       <c r="M35" s="16" t="s">
@@ -2845,7 +2845,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>1</v>
@@ -2857,7 +2857,7 @@
         <v>181</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L36" s="17"/>
       <c r="M36" s="16" t="s">
@@ -2891,7 +2891,7 @@
         <v>26</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>1</v>
@@ -2903,7 +2903,7 @@
         <v>181</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L37" s="17"/>
       <c r="M37" s="16" t="s">
@@ -2937,7 +2937,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>5</v>
@@ -2983,7 +2983,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>5</v>
@@ -3029,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>5</v>
@@ -3075,7 +3075,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>5</v>
@@ -3121,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H42" s="17" t="s">
         <v>5</v>
@@ -3167,7 +3167,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>5</v>
@@ -3213,7 +3213,7 @@
         <v>2</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H44" s="17" t="s">
         <v>5</v>
@@ -3259,7 +3259,7 @@
         <v>2</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H45" s="17" t="s">
         <v>5</v>
@@ -3305,7 +3305,7 @@
         <v>2</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H46" s="17" t="s">
         <v>5</v>
@@ -3351,7 +3351,7 @@
         <v>2</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H47" s="17" t="s">
         <v>5</v>
@@ -3397,7 +3397,7 @@
         <v>2</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H48" s="17" t="s">
         <v>5</v>
@@ -3443,7 +3443,7 @@
         <v>2</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H49" s="17" t="s">
         <v>5</v>
@@ -3489,7 +3489,7 @@
         <v>2</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H50" s="17" t="s">
         <v>5</v>
@@ -3535,7 +3535,7 @@
         <v>2</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H51" s="17" t="s">
         <v>5</v>
@@ -3581,7 +3581,7 @@
         <v>2</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H52" s="17" t="s">
         <v>5</v>
@@ -3627,7 +3627,7 @@
         <v>2</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H53" s="17" t="s">
         <v>5</v>
@@ -3673,7 +3673,7 @@
         <v>2</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H54" s="17" t="s">
         <v>5</v>
@@ -3719,7 +3719,7 @@
         <v>2</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H55" s="17" t="s">
         <v>5</v>
@@ -3765,7 +3765,7 @@
         <v>2</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H56" s="17" t="s">
         <v>5</v>
@@ -3811,7 +3811,7 @@
         <v>2</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H57" s="17" t="s">
         <v>5</v>
@@ -3857,7 +3857,7 @@
         <v>2</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H58" s="17" t="s">
         <v>5</v>
@@ -3903,7 +3903,7 @@
         <v>2</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H59" s="17" t="s">
         <v>5</v>
@@ -3949,7 +3949,7 @@
         <v>2</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H60" s="17" t="s">
         <v>1</v>
@@ -3961,7 +3961,7 @@
         <v>186</v>
       </c>
       <c r="K60" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L60" s="16"/>
       <c r="M60" s="16" t="s">
@@ -3995,7 +3995,7 @@
         <v>2</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H61" s="17" t="s">
         <v>5</v>
@@ -4041,7 +4041,7 @@
         <v>2</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H62" s="17" t="s">
         <v>1</v>
@@ -4053,7 +4053,7 @@
         <v>186</v>
       </c>
       <c r="K62" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L62" s="16"/>
       <c r="M62" s="16" t="s">
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H63" s="17" t="s">
         <v>5</v>
@@ -4133,7 +4133,7 @@
         <v>2</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H64" s="17" t="s">
         <v>1</v>
@@ -4145,7 +4145,7 @@
         <v>186</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L64" s="16"/>
       <c r="M64" s="16" t="s">
@@ -4179,7 +4179,7 @@
         <v>2</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H65" s="17" t="s">
         <v>1</v>
@@ -4191,7 +4191,7 @@
         <v>186</v>
       </c>
       <c r="K65" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L65" s="16"/>
       <c r="M65" s="16" t="s">
@@ -4225,7 +4225,7 @@
         <v>2</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H66" s="17" t="s">
         <v>5</v>
@@ -4271,7 +4271,7 @@
         <v>2</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H67" s="17" t="s">
         <v>1</v>
@@ -4283,7 +4283,7 @@
         <v>186</v>
       </c>
       <c r="K67" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L67" s="16"/>
       <c r="M67" s="16" t="s">
@@ -4317,7 +4317,7 @@
         <v>2</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H68" s="17" t="s">
         <v>5</v>
@@ -4363,7 +4363,7 @@
         <v>2</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H69" s="17" t="s">
         <v>1</v>
@@ -4375,7 +4375,7 @@
         <v>186</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L69" s="16"/>
       <c r="M69" s="16" t="s">
@@ -4409,7 +4409,7 @@
         <v>2</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H70" s="17" t="s">
         <v>5</v>
@@ -4455,7 +4455,7 @@
         <v>2</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H71" s="17" t="s">
         <v>5</v>
@@ -4501,7 +4501,7 @@
         <v>2</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H72" s="17" t="s">
         <v>5</v>
@@ -4547,7 +4547,7 @@
         <v>2</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H73" s="17" t="s">
         <v>1</v>
@@ -4559,7 +4559,7 @@
         <v>186</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L73" s="16"/>
       <c r="M73" s="16" t="s">
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H74" s="20" t="s">
         <v>1</v>
@@ -4605,7 +4605,7 @@
         <v>182</v>
       </c>
       <c r="K74" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L74" s="16"/>
       <c r="M74" s="16" t="s">
@@ -4639,7 +4639,7 @@
         <v>2</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H75" s="20" t="s">
         <v>1</v>
@@ -4651,7 +4651,7 @@
         <v>182</v>
       </c>
       <c r="K75" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L75" s="16"/>
       <c r="M75" s="16" t="s">
@@ -4685,7 +4685,7 @@
         <v>2</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H76" s="20" t="s">
         <v>1</v>
@@ -4697,7 +4697,7 @@
         <v>182</v>
       </c>
       <c r="K76" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L76" s="16"/>
       <c r="M76" s="16" t="s">
@@ -4731,7 +4731,7 @@
         <v>2</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H77" s="20" t="s">
         <v>1</v>
@@ -4743,7 +4743,7 @@
         <v>183</v>
       </c>
       <c r="K77" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L77" s="16"/>
       <c r="M77" s="16" t="s">
@@ -4777,7 +4777,7 @@
         <v>26</v>
       </c>
       <c r="G78" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H78" s="20" t="s">
         <v>1</v>
@@ -4789,7 +4789,7 @@
         <v>183</v>
       </c>
       <c r="K78" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L78" s="16"/>
       <c r="M78" s="16" t="s">
@@ -4823,7 +4823,7 @@
         <v>2</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H79" s="20" t="s">
         <v>1</v>
@@ -4835,7 +4835,7 @@
         <v>183</v>
       </c>
       <c r="K79" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L79" s="16"/>
       <c r="M79" s="16" t="s">
@@ -4869,7 +4869,7 @@
         <v>2</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H80" s="20" t="s">
         <v>1</v>
@@ -4881,7 +4881,7 @@
         <v>183</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L80" s="16"/>
       <c r="M80" s="16" t="s">
@@ -4915,7 +4915,7 @@
         <v>25</v>
       </c>
       <c r="G81" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H81" s="20" t="s">
         <v>1</v>
@@ -4927,7 +4927,7 @@
         <v>183</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L81" s="16"/>
       <c r="M81" s="16" t="s">
@@ -4961,7 +4961,7 @@
         <v>38</v>
       </c>
       <c r="G82" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H82" s="20" t="s">
         <v>1</v>
@@ -4973,7 +4973,7 @@
         <v>183</v>
       </c>
       <c r="K82" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L82" s="16"/>
       <c r="M82" s="16" t="s">
@@ -5007,7 +5007,7 @@
         <v>32</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H83" s="20" t="s">
         <v>1</v>
@@ -5019,7 +5019,7 @@
         <v>183</v>
       </c>
       <c r="K83" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L83" s="16"/>
       <c r="M83" s="16" t="s">
@@ -5053,7 +5053,7 @@
         <v>2</v>
       </c>
       <c r="G84" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H84" s="20" t="s">
         <v>1</v>
@@ -5065,7 +5065,7 @@
         <v>183</v>
       </c>
       <c r="K84" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L84" s="16"/>
       <c r="M84" s="16" t="s">
@@ -5099,7 +5099,7 @@
         <v>2</v>
       </c>
       <c r="G85" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H85" s="20" t="s">
         <v>1</v>
@@ -5111,7 +5111,7 @@
         <v>183</v>
       </c>
       <c r="K85" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L85" s="16"/>
       <c r="M85" s="16" t="s">
@@ -5145,7 +5145,7 @@
         <v>49</v>
       </c>
       <c r="G86" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H86" s="20" t="s">
         <v>1</v>
@@ -5157,7 +5157,7 @@
         <v>183</v>
       </c>
       <c r="K86" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L86" s="16"/>
       <c r="M86" s="16" t="s">
@@ -5191,7 +5191,7 @@
         <v>2</v>
       </c>
       <c r="G87" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H87" s="20" t="s">
         <v>1</v>
@@ -5203,7 +5203,7 @@
         <v>55</v>
       </c>
       <c r="K87" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L87" s="16"/>
       <c r="M87" s="16" t="s">
@@ -5237,7 +5237,7 @@
         <v>32</v>
       </c>
       <c r="G88" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H88" s="20" t="s">
         <v>1</v>
@@ -5249,7 +5249,7 @@
         <v>55</v>
       </c>
       <c r="K88" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L88" s="16"/>
       <c r="M88" s="16" t="s">
@@ -5283,7 +5283,7 @@
         <v>35</v>
       </c>
       <c r="G89" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H89" s="20" t="s">
         <v>1</v>
@@ -5295,7 +5295,7 @@
         <v>55</v>
       </c>
       <c r="K89" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L89" s="16"/>
       <c r="M89" s="16" t="s">
@@ -5329,7 +5329,7 @@
         <v>35</v>
       </c>
       <c r="G90" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H90" s="20" t="s">
         <v>1</v>
@@ -5341,7 +5341,7 @@
         <v>55</v>
       </c>
       <c r="K90" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L90" s="16"/>
       <c r="M90" s="16" t="s">
@@ -5375,7 +5375,7 @@
         <v>35</v>
       </c>
       <c r="G91" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H91" s="20" t="s">
         <v>1</v>
@@ -5387,7 +5387,7 @@
         <v>187</v>
       </c>
       <c r="K91" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L91" s="16"/>
       <c r="M91" s="16" t="s">
@@ -5421,7 +5421,7 @@
         <v>35</v>
       </c>
       <c r="G92" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H92" s="20" t="s">
         <v>1</v>
@@ -5433,7 +5433,7 @@
         <v>187</v>
       </c>
       <c r="K92" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L92" s="29"/>
       <c r="M92" s="16" t="s">
@@ -5467,7 +5467,7 @@
         <v>26</v>
       </c>
       <c r="G93" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H93" s="20" t="s">
         <v>1</v>
@@ -5479,7 +5479,7 @@
         <v>187</v>
       </c>
       <c r="K93" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L93" s="16"/>
       <c r="M93" s="16" t="s">
@@ -5513,7 +5513,7 @@
         <v>35</v>
       </c>
       <c r="G94" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H94" s="20" t="s">
         <v>1</v>
@@ -5525,7 +5525,7 @@
         <v>187</v>
       </c>
       <c r="K94" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L94" s="16"/>
       <c r="M94" s="16" t="s">
@@ -5559,7 +5559,7 @@
         <v>2</v>
       </c>
       <c r="G95" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H95" s="20" t="s">
         <v>1</v>
@@ -5571,7 +5571,7 @@
         <v>187</v>
       </c>
       <c r="K95" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L95" s="17"/>
       <c r="M95" s="16" t="s">
@@ -5605,7 +5605,7 @@
         <v>38</v>
       </c>
       <c r="G96" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H96" s="20" t="s">
         <v>1</v>
@@ -5617,7 +5617,7 @@
         <v>187</v>
       </c>
       <c r="K96" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L96" s="16"/>
       <c r="M96" s="16" t="s">
@@ -5651,7 +5651,7 @@
         <v>2</v>
       </c>
       <c r="G97" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H97" s="20" t="s">
         <v>1</v>
@@ -5663,7 +5663,7 @@
         <v>187</v>
       </c>
       <c r="K97" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L97" s="16"/>
       <c r="M97" s="16" t="s">
@@ -5697,7 +5697,7 @@
         <v>56</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H98" s="20" t="s">
         <v>1</v>
@@ -5709,7 +5709,7 @@
         <v>187</v>
       </c>
       <c r="K98" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L98" s="16"/>
       <c r="M98" s="16" t="s">
@@ -5743,7 +5743,7 @@
         <v>2</v>
       </c>
       <c r="G99" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H99" s="20" t="s">
         <v>1</v>
@@ -5755,7 +5755,7 @@
         <v>187</v>
       </c>
       <c r="K99" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L99" s="16"/>
       <c r="M99" s="16" t="s">
@@ -5789,7 +5789,7 @@
         <v>2</v>
       </c>
       <c r="G100" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H100" s="20" t="s">
         <v>1</v>
@@ -5801,7 +5801,7 @@
         <v>187</v>
       </c>
       <c r="K100" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L100" s="16"/>
       <c r="M100" s="16" t="s">
@@ -5835,7 +5835,7 @@
         <v>2</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H101" s="20" t="s">
         <v>1</v>
@@ -5847,7 +5847,7 @@
         <v>187</v>
       </c>
       <c r="K101" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L101" s="16"/>
       <c r="M101" s="16" t="s">
@@ -5881,7 +5881,7 @@
         <v>26</v>
       </c>
       <c r="G102" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H102" s="20" t="s">
         <v>1</v>
@@ -5893,7 +5893,7 @@
         <v>187</v>
       </c>
       <c r="K102" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L102" s="16"/>
       <c r="M102" s="16" t="s">
@@ -5927,7 +5927,7 @@
         <v>2</v>
       </c>
       <c r="G103" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H103" s="20" t="s">
         <v>1</v>
@@ -5939,7 +5939,7 @@
         <v>187</v>
       </c>
       <c r="K103" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L103" s="16"/>
       <c r="M103" s="16" t="s">
@@ -5973,7 +5973,7 @@
         <v>2</v>
       </c>
       <c r="G104" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H104" s="20" t="s">
         <v>1</v>
@@ -5985,7 +5985,7 @@
         <v>187</v>
       </c>
       <c r="K104" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L104" s="16"/>
       <c r="M104" s="16" t="s">
@@ -6019,7 +6019,7 @@
         <v>2</v>
       </c>
       <c r="G105" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H105" s="20" t="s">
         <v>1</v>
@@ -6031,7 +6031,7 @@
         <v>187</v>
       </c>
       <c r="K105" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L105" s="16"/>
       <c r="M105" s="16" t="s">
@@ -6065,7 +6065,7 @@
         <v>60</v>
       </c>
       <c r="G106" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H106" s="20" t="s">
         <v>1</v>
@@ -6077,7 +6077,7 @@
         <v>187</v>
       </c>
       <c r="K106" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L106" s="16"/>
       <c r="M106" s="16" t="s">
@@ -6111,7 +6111,7 @@
         <v>2</v>
       </c>
       <c r="G107" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H107" s="20" t="s">
         <v>1</v>
@@ -6123,7 +6123,7 @@
         <v>187</v>
       </c>
       <c r="K107" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L107" s="16"/>
       <c r="M107" s="16" t="s">
@@ -6157,7 +6157,7 @@
         <v>62</v>
       </c>
       <c r="G108" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H108" s="20" t="s">
         <v>1</v>
@@ -6169,7 +6169,7 @@
         <v>187</v>
       </c>
       <c r="K108" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L108" s="16"/>
       <c r="M108" s="16" t="s">
@@ -6203,7 +6203,7 @@
         <v>2</v>
       </c>
       <c r="G109" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H109" s="20" t="s">
         <v>1</v>
@@ -6215,7 +6215,7 @@
         <v>57</v>
       </c>
       <c r="K109" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L109" s="16"/>
       <c r="M109" s="16" t="s">
@@ -6249,7 +6249,7 @@
         <v>56</v>
       </c>
       <c r="G110" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H110" s="20" t="s">
         <v>1</v>
@@ -6261,7 +6261,7 @@
         <v>57</v>
       </c>
       <c r="K110" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L110" s="20"/>
       <c r="M110" s="16" t="s">
@@ -6295,7 +6295,7 @@
         <v>2</v>
       </c>
       <c r="G111" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H111" s="20" t="s">
         <v>1</v>
@@ -6307,7 +6307,7 @@
         <v>57</v>
       </c>
       <c r="K111" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L111" s="20"/>
       <c r="M111" s="16" t="s">
@@ -6341,7 +6341,7 @@
         <v>2</v>
       </c>
       <c r="G112" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H112" s="20" t="s">
         <v>1</v>
@@ -6353,7 +6353,7 @@
         <v>57</v>
       </c>
       <c r="K112" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L112" s="20"/>
       <c r="M112" s="16" t="s">
@@ -6387,7 +6387,7 @@
         <v>2</v>
       </c>
       <c r="G113" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H113" s="20" t="s">
         <v>1</v>
@@ -6399,7 +6399,7 @@
         <v>57</v>
       </c>
       <c r="K113" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L113" s="20"/>
       <c r="M113" s="16" t="s">
@@ -6433,7 +6433,7 @@
         <v>2</v>
       </c>
       <c r="G114" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H114" s="20" t="s">
         <v>1</v>
@@ -6445,7 +6445,7 @@
         <v>57</v>
       </c>
       <c r="K114" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L114" s="20"/>
       <c r="M114" s="16" t="s">
@@ -6479,7 +6479,7 @@
         <v>2</v>
       </c>
       <c r="G115" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H115" s="20" t="s">
         <v>1</v>
@@ -6491,7 +6491,7 @@
         <v>57</v>
       </c>
       <c r="K115" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L115" s="20"/>
       <c r="M115" s="16" t="s">
@@ -6525,7 +6525,7 @@
         <v>2</v>
       </c>
       <c r="G116" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H116" s="20" t="s">
         <v>1</v>
@@ -6537,7 +6537,7 @@
         <v>57</v>
       </c>
       <c r="K116" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L116" s="20"/>
       <c r="M116" s="16" t="s">
@@ -6571,7 +6571,7 @@
         <v>26</v>
       </c>
       <c r="G117" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H117" s="20" t="s">
         <v>1</v>
@@ -6583,7 +6583,7 @@
         <v>57</v>
       </c>
       <c r="K117" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L117" s="20"/>
       <c r="M117" s="16" t="s">
@@ -6617,7 +6617,7 @@
         <v>26</v>
       </c>
       <c r="G118" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H118" s="20" t="s">
         <v>1</v>
@@ -6629,7 +6629,7 @@
         <v>57</v>
       </c>
       <c r="K118" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L118" s="20"/>
       <c r="M118" s="16" t="s">
@@ -6663,7 +6663,7 @@
         <v>2</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H119" s="20" t="s">
         <v>1</v>
@@ -6675,7 +6675,7 @@
         <v>57</v>
       </c>
       <c r="K119" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L119" s="20"/>
       <c r="M119" s="16" t="s">
@@ -6709,7 +6709,7 @@
         <v>2</v>
       </c>
       <c r="G120" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H120" s="20" t="s">
         <v>5</v>
@@ -6755,7 +6755,7 @@
         <v>2</v>
       </c>
       <c r="G121" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H121" s="20" t="s">
         <v>5</v>
@@ -6801,7 +6801,7 @@
         <v>2</v>
       </c>
       <c r="G122" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H122" s="20" t="s">
         <v>5</v>
@@ -6847,7 +6847,7 @@
         <v>2</v>
       </c>
       <c r="G123" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H123" s="20" t="s">
         <v>5</v>
@@ -6893,7 +6893,7 @@
         <v>2</v>
       </c>
       <c r="G124" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H124" s="20" t="s">
         <v>1</v>
@@ -6905,7 +6905,7 @@
         <v>70</v>
       </c>
       <c r="K124" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L124" s="20"/>
       <c r="M124" s="16" t="s">
@@ -6939,7 +6939,7 @@
         <v>2</v>
       </c>
       <c r="G125" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H125" s="20" t="s">
         <v>1</v>
@@ -6951,7 +6951,7 @@
         <v>70</v>
       </c>
       <c r="K125" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L125" s="20"/>
       <c r="M125" s="16" t="s">
@@ -6985,7 +6985,7 @@
         <v>2</v>
       </c>
       <c r="G126" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H126" s="20" t="s">
         <v>1</v>
@@ -6997,7 +6997,7 @@
         <v>70</v>
       </c>
       <c r="K126" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L126" s="20"/>
       <c r="M126" s="16" t="s">
@@ -7031,7 +7031,7 @@
         <v>2</v>
       </c>
       <c r="G127" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H127" s="20" t="s">
         <v>1</v>
@@ -7043,7 +7043,7 @@
         <v>70</v>
       </c>
       <c r="K127" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L127" s="20"/>
       <c r="M127" s="16" t="s">
@@ -7077,7 +7077,7 @@
         <v>2</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H128" s="20" t="s">
         <v>1</v>
@@ -7089,7 +7089,7 @@
         <v>70</v>
       </c>
       <c r="K128" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L128" s="20"/>
       <c r="M128" s="16" t="s">
@@ -7123,7 +7123,7 @@
         <v>2</v>
       </c>
       <c r="G129" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H129" s="20" t="s">
         <v>1</v>
@@ -7135,7 +7135,7 @@
         <v>73</v>
       </c>
       <c r="K129" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L129" s="20"/>
       <c r="M129" s="16" t="s">
@@ -7169,7 +7169,7 @@
         <v>2</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H130" s="20" t="s">
         <v>1</v>
@@ -7181,7 +7181,7 @@
         <v>73</v>
       </c>
       <c r="K130" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L130" s="20"/>
       <c r="M130" s="16" t="s">
@@ -7215,7 +7215,7 @@
         <v>2</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H131" s="20" t="s">
         <v>1</v>
@@ -7227,7 +7227,7 @@
         <v>73</v>
       </c>
       <c r="K131" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L131" s="20"/>
       <c r="M131" s="16" t="s">
@@ -7261,7 +7261,7 @@
         <v>2</v>
       </c>
       <c r="G132" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H132" s="20" t="s">
         <v>1</v>
@@ -7273,7 +7273,7 @@
         <v>73</v>
       </c>
       <c r="K132" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L132" s="20"/>
       <c r="M132" s="16" t="s">
@@ -7307,7 +7307,7 @@
         <v>2</v>
       </c>
       <c r="G133" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H133" s="20" t="s">
         <v>1</v>
@@ -7319,7 +7319,7 @@
         <v>73</v>
       </c>
       <c r="K133" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L133" s="20"/>
       <c r="M133" s="16" t="s">
@@ -7353,7 +7353,7 @@
         <v>2</v>
       </c>
       <c r="G134" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H134" s="20" t="s">
         <v>1</v>
@@ -7365,7 +7365,7 @@
         <v>73</v>
       </c>
       <c r="K134" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L134" s="20"/>
       <c r="M134" s="16" t="s">
@@ -7399,7 +7399,7 @@
         <v>2</v>
       </c>
       <c r="G135" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H135" s="20" t="s">
         <v>1</v>
@@ -7411,7 +7411,7 @@
         <v>73</v>
       </c>
       <c r="K135" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L135" s="20"/>
       <c r="M135" s="16" t="s">
@@ -7445,7 +7445,7 @@
         <v>33</v>
       </c>
       <c r="G136" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H136" s="20" t="s">
         <v>1</v>
@@ -7457,7 +7457,7 @@
         <v>73</v>
       </c>
       <c r="K136" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L136" s="20"/>
       <c r="M136" s="16" t="s">
@@ -7491,7 +7491,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H137" s="20" t="s">
         <v>5</v>
@@ -7537,7 +7537,7 @@
         <v>2</v>
       </c>
       <c r="G138" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H138" s="20" t="s">
         <v>5</v>
@@ -7583,7 +7583,7 @@
         <v>2</v>
       </c>
       <c r="G139" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H139" s="20" t="s">
         <v>5</v>
@@ -7629,7 +7629,7 @@
         <v>2</v>
       </c>
       <c r="G140" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H140" s="20" t="s">
         <v>5</v>
@@ -7675,7 +7675,7 @@
         <v>2</v>
       </c>
       <c r="G141" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H141" s="20" t="s">
         <v>5</v>
@@ -7721,7 +7721,7 @@
         <v>2</v>
       </c>
       <c r="G142" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H142" s="20" t="s">
         <v>5</v>
@@ -7767,7 +7767,7 @@
         <v>2</v>
       </c>
       <c r="G143" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H143" s="20" t="s">
         <v>5</v>
@@ -7813,7 +7813,7 @@
         <v>2</v>
       </c>
       <c r="G144" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H144" s="20" t="s">
         <v>5</v>
@@ -7859,7 +7859,7 @@
         <v>2</v>
       </c>
       <c r="G145" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H145" s="20" t="s">
         <v>5</v>
@@ -7905,7 +7905,7 @@
         <v>2</v>
       </c>
       <c r="G146" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H146" s="20" t="s">
         <v>5</v>
@@ -7951,7 +7951,7 @@
         <v>2</v>
       </c>
       <c r="G147" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H147" s="20" t="s">
         <v>5</v>
@@ -7997,7 +7997,7 @@
         <v>2</v>
       </c>
       <c r="G148" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H148" s="20" t="s">
         <v>5</v>
@@ -8043,7 +8043,7 @@
         <v>2</v>
       </c>
       <c r="G149" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H149" s="20" t="s">
         <v>5</v>
@@ -8089,7 +8089,7 @@
         <v>2</v>
       </c>
       <c r="G150" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H150" s="20" t="s">
         <v>5</v>
@@ -8135,7 +8135,7 @@
         <v>2</v>
       </c>
       <c r="G151" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H151" s="20" t="s">
         <v>5</v>
@@ -8181,7 +8181,7 @@
         <v>2</v>
       </c>
       <c r="G152" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H152" s="20" t="s">
         <v>5</v>
@@ -8227,7 +8227,7 @@
         <v>2</v>
       </c>
       <c r="G153" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H153" s="20" t="s">
         <v>5</v>
@@ -8273,7 +8273,7 @@
         <v>2</v>
       </c>
       <c r="G154" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H154" s="20" t="s">
         <v>5</v>
@@ -8319,7 +8319,7 @@
         <v>2</v>
       </c>
       <c r="G155" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H155" s="20" t="s">
         <v>5</v>
@@ -8365,7 +8365,7 @@
         <v>2</v>
       </c>
       <c r="G156" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H156" s="20" t="s">
         <v>5</v>
@@ -8411,7 +8411,7 @@
         <v>2</v>
       </c>
       <c r="G157" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H157" s="20" t="s">
         <v>5</v>
@@ -8457,7 +8457,7 @@
         <v>2</v>
       </c>
       <c r="G158" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H158" s="20" t="s">
         <v>5</v>
@@ -8503,7 +8503,7 @@
         <v>2</v>
       </c>
       <c r="G159" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H159" s="20" t="s">
         <v>5</v>
@@ -8549,7 +8549,7 @@
         <v>2</v>
       </c>
       <c r="G160" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H160" s="20" t="s">
         <v>5</v>
@@ -8595,7 +8595,7 @@
         <v>2</v>
       </c>
       <c r="G161" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H161" s="20" t="s">
         <v>5</v>
@@ -8641,7 +8641,7 @@
         <v>2</v>
       </c>
       <c r="G162" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H162" s="20" t="s">
         <v>5</v>
@@ -8687,7 +8687,7 @@
         <v>2</v>
       </c>
       <c r="G163" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H163" s="20" t="s">
         <v>5</v>
@@ -8733,7 +8733,7 @@
         <v>2</v>
       </c>
       <c r="G164" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H164" s="20" t="s">
         <v>5</v>
@@ -8779,7 +8779,7 @@
         <v>2</v>
       </c>
       <c r="G165" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H165" s="20" t="s">
         <v>5</v>
@@ -8825,7 +8825,7 @@
         <v>2</v>
       </c>
       <c r="G166" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H166" s="20" t="s">
         <v>5</v>
@@ -8871,7 +8871,7 @@
         <v>2</v>
       </c>
       <c r="G167" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H167" s="20" t="s">
         <v>5</v>
@@ -8917,7 +8917,7 @@
         <v>2</v>
       </c>
       <c r="G168" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H168" s="20" t="s">
         <v>5</v>
@@ -8963,7 +8963,7 @@
         <v>2</v>
       </c>
       <c r="G169" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H169" s="20" t="s">
         <v>5</v>
@@ -9009,7 +9009,7 @@
         <v>2</v>
       </c>
       <c r="G170" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H170" s="20" t="s">
         <v>5</v>
@@ -9055,7 +9055,7 @@
         <v>2</v>
       </c>
       <c r="G171" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H171" s="20" t="s">
         <v>5</v>
@@ -9101,7 +9101,7 @@
         <v>2</v>
       </c>
       <c r="G172" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H172" s="20" t="s">
         <v>5</v>
@@ -9147,7 +9147,7 @@
         <v>2</v>
       </c>
       <c r="G173" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H173" s="20" t="s">
         <v>5</v>
@@ -9193,7 +9193,7 @@
         <v>2</v>
       </c>
       <c r="G174" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H174" s="20" t="s">
         <v>5</v>
@@ -9239,7 +9239,7 @@
         <v>2</v>
       </c>
       <c r="G175" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H175" s="20" t="s">
         <v>5</v>
@@ -9285,7 +9285,7 @@
         <v>2</v>
       </c>
       <c r="G176" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H176" s="20" t="s">
         <v>5</v>
@@ -9331,7 +9331,7 @@
         <v>2</v>
       </c>
       <c r="G177" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H177" s="32" t="s">
         <v>1</v>
@@ -9343,7 +9343,7 @@
         <v>184</v>
       </c>
       <c r="K177" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L177" s="11"/>
       <c r="M177" s="26" t="s">
@@ -9377,7 +9377,7 @@
         <v>2</v>
       </c>
       <c r="G178" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H178" s="30" t="s">
         <v>1</v>
@@ -9389,7 +9389,7 @@
         <v>84</v>
       </c>
       <c r="K178" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L178" s="11"/>
       <c r="M178" s="20" t="s">
@@ -9423,7 +9423,7 @@
         <v>83</v>
       </c>
       <c r="G179" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H179" s="30" t="s">
         <v>1</v>
@@ -9435,7 +9435,7 @@
         <v>84</v>
       </c>
       <c r="K179" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L179" s="11"/>
       <c r="M179" s="20" t="s">
@@ -9469,7 +9469,7 @@
         <v>2</v>
       </c>
       <c r="G180" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H180" s="30" t="s">
         <v>1</v>
@@ -9481,7 +9481,7 @@
         <v>188</v>
       </c>
       <c r="K180" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L180" s="11"/>
       <c r="M180" s="20" t="s">
@@ -9515,7 +9515,7 @@
         <v>86</v>
       </c>
       <c r="G181" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H181" s="32" t="s">
         <v>1</v>
@@ -9527,7 +9527,7 @@
         <v>188</v>
       </c>
       <c r="K181" s="26" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L181" s="11"/>
       <c r="M181" s="26" t="s">
@@ -9561,7 +9561,7 @@
         <v>2</v>
       </c>
       <c r="G182" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H182" s="30" t="s">
         <v>1</v>
@@ -9573,7 +9573,7 @@
         <v>188</v>
       </c>
       <c r="K182" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L182" s="11"/>
       <c r="M182" s="30" t="s">
@@ -9607,7 +9607,7 @@
         <v>88</v>
       </c>
       <c r="G183" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H183" s="30" t="s">
         <v>1</v>
@@ -9619,7 +9619,7 @@
         <v>188</v>
       </c>
       <c r="K183" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L183" s="11"/>
       <c r="M183" s="30" t="s">
@@ -9653,7 +9653,7 @@
         <v>2</v>
       </c>
       <c r="G184" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H184" s="30" t="s">
         <v>1</v>
@@ -9665,7 +9665,7 @@
         <v>185</v>
       </c>
       <c r="K184" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L184" s="11"/>
       <c r="M184" s="30" t="s">
@@ -9699,7 +9699,7 @@
         <v>2</v>
       </c>
       <c r="G185" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H185" s="34" t="s">
         <v>5</v>
@@ -9745,7 +9745,7 @@
         <v>2</v>
       </c>
       <c r="G186" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H186" s="34" t="s">
         <v>5</v>
@@ -9791,7 +9791,7 @@
         <v>2</v>
       </c>
       <c r="G187" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H187" s="34" t="s">
         <v>5</v>
@@ -9837,7 +9837,7 @@
         <v>2</v>
       </c>
       <c r="G188" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H188" s="34" t="s">
         <v>5</v>
@@ -9883,7 +9883,7 @@
         <v>2</v>
       </c>
       <c r="G189" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H189" s="34" t="s">
         <v>5</v>
@@ -9929,7 +9929,7 @@
         <v>2</v>
       </c>
       <c r="G190" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H190" s="34" t="s">
         <v>5</v>
@@ -9975,7 +9975,7 @@
         <v>2</v>
       </c>
       <c r="G191" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H191" s="34" t="s">
         <v>5</v>
@@ -10021,7 +10021,7 @@
         <v>2</v>
       </c>
       <c r="G192" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H192" s="34" t="s">
         <v>5</v>
@@ -10067,7 +10067,7 @@
         <v>2</v>
       </c>
       <c r="G193" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H193" s="34" t="s">
         <v>5</v>
@@ -10113,7 +10113,7 @@
         <v>2</v>
       </c>
       <c r="G194" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H194" s="34" t="s">
         <v>5</v>
@@ -10141,13 +10141,13 @@
     </row>
     <row r="195" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="40" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B195" s="40" t="s">
         <v>21</v>
       </c>
       <c r="C195" s="40" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D195" s="40" t="s">
         <v>23</v>
@@ -10156,17 +10156,17 @@
         <v>22</v>
       </c>
       <c r="G195" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H195" s="40" t="s">
         <v>1</v>
       </c>
       <c r="I195" s="41"/>
       <c r="J195" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K195" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="O195" s="40">
         <v>30125371</v>
@@ -10186,7 +10186,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:I9"/>
+      <selection activeCell="H12" sqref="H12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10286,7 +10286,7 @@
         <v>188</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>189</v>
@@ -10298,16 +10298,16 @@
         <v>185</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>183</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>